<commit_message>
Primer commit del proyecto Aplicativo_Web_Pro
</commit_message>
<xml_diff>
--- a/templates/configuracion/Seguridad/Plantillas/Plantilla cargue Funcionalidades.xlsx
+++ b/templates/configuracion/Seguridad/Plantillas/Plantilla cargue Funcionalidades.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca2052e6604c4b79/Proyectos/Aplicativo_Web_Pro/templates/configuracion/Seguridad/Plantillas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{4480893A-436D-49D9-A648-596BA64066B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EA0B5A3-4DB0-45BD-B946-FE9EB84301E9}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{4480893A-436D-49D9-A648-596BA64066B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2B2B5FA-7213-41A9-9708-2446448A4FCB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4E3B284B-0EA2-4AA5-9D7B-E62466E62097}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plantilla!$A$1:$H$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>Nombre</t>
   </si>
@@ -68,9 +71,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>20.06.2025</t>
-  </si>
-  <si>
     <t>mySiss</t>
   </si>
   <si>
@@ -101,36 +101,15 @@
     <t>AH002</t>
   </si>
   <si>
-    <t>Configuración</t>
-  </si>
-  <si>
-    <t>Crear configuración</t>
-  </si>
-  <si>
-    <t>Modificar configuración</t>
-  </si>
-  <si>
     <t>AH003</t>
   </si>
   <si>
-    <t>Ver configuración</t>
-  </si>
-  <si>
-    <t>Proceso</t>
-  </si>
-  <si>
     <t>AH004</t>
   </si>
   <si>
-    <t>Procesar honorarios</t>
-  </si>
-  <si>
     <t>AH005</t>
   </si>
   <si>
-    <t>Generar reportes</t>
-  </si>
-  <si>
     <t>MH002</t>
   </si>
   <si>
@@ -138,12 +117,36 @@
   </si>
   <si>
     <t>FH004</t>
+  </si>
+  <si>
+    <t>Preliquidacion</t>
+  </si>
+  <si>
+    <t>Liquidacion</t>
+  </si>
+  <si>
+    <t>Radicacion facturas</t>
+  </si>
+  <si>
+    <t>Validación facturas</t>
+  </si>
+  <si>
+    <t>Crear preliquidación</t>
+  </si>
+  <si>
+    <t>filtrar preliquidación</t>
+  </si>
+  <si>
+    <t>radicar preliquidación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,8 +176,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,20 +516,21 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A1:XFD11"/>
+      <selection activeCell="C8" sqref="C8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -559,199 +564,215 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
+      <c r="E2" s="1">
+        <f ca="1">+TODAY()</f>
+        <v>45840</v>
+      </c>
+      <c r="F2" s="1">
+        <f ca="1">+TODAY()</f>
+        <v>45840</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:F12" ca="1" si="0">+TODAY()</f>
+        <v>45840</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
+      <c r="E7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -759,80 +780,87 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
+      <c r="E10" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45840</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H12" xr:uid="{6390E410-44CD-4D6A-AB7B-EE07051BF53D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>